<commit_message>
refactor(csv): refactored CSV handling to add writing as well as reading
</commit_message>
<xml_diff>
--- a/Data/ExcelDynamic.Xlsx
+++ b/Data/ExcelDynamic.Xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="test" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001" fullCalcOnLoad="1" fullPrecision="1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,91 +20,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Surname</t>
-  </si>
-  <si>
-    <t>DOB</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Colour</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Wanted?</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>12-11-1981</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>f511</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Janet</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>F502</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanted?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bobbie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-11-1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F502</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="14">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,7 +120,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="1" diagonalDown="1">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -129,39 +128,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="1" applyProtection="1" applyAlignment="1"/>
-    <xf numFmtId="43" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="41" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="44" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="42" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="9" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1"/>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -273,29 +297,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr xr2 ">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.58" customWidth="1" style="1"/>
-    <col min="2" max="2" width="8.8" customWidth="1" style="1"/>
-    <col min="3" max="3" width="17.99" customWidth="1" style="2"/>
-    <col min="4" max="4" width="4.76" customWidth="1" style="1"/>
-    <col min="5" max="5" width="7.54" customWidth="1" style="1"/>
-    <col min="6" max="7" width="6.71" customWidth="1" style="1"/>
-    <col min="8" max="8" width="8.67" customWidth="1" style="3"/>
-    <col min="10" max="16384" width="11.52" customWidth="1" style="1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -321,7 +345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="12.8">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -347,17 +371,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" ht="12.8">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="4" t="n">
         <v>31213</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -369,8 +393,8 @@
       <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5">
-        <f>FALSE()</f>
+      <c r="H3" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -383,9 +407,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=EPPlusLicense.txt>This workbook was created with the EPPlus library, licensed to Ryan Weavers under the Polyform Noncommercial license, see https://polyformproject.org/licenses/noncommercial/1.0.0
-For more information about EPPlus, see https://epplussoftware.com/
-
 </file>
</xml_diff>

<commit_message>
reverted back to previous version due to complexity issues
</commit_message>
<xml_diff>
--- a/Data/ExcelDynamic.Xlsx
+++ b/Data/ExcelDynamic.Xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="test" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="ExcelDynamic" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001" fullCalcOnLoad="1" fullPrecision="1"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -20,91 +20,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Surname</t>
-  </si>
-  <si>
-    <t>DOB</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Colour</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Wanted?</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>12-11-1981</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>f511</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Janet</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>F502</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanted?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-11-1981</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f511</t>
+  </si>
+  <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F502</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="14">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,7 +120,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="1" diagonalDown="1">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -129,39 +128,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="1" applyProtection="1" applyAlignment="1"/>
-    <xf numFmtId="43" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="41" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="44" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="42" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="9" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1"/>
-    <xf numFmtId="164" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" borderId="0" applyBorder="0" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -273,7 +297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr xr2 ">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -285,17 +309,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="11.58" customWidth="1" style="1"/>
-    <col min="2" max="2" width="8.8" customWidth="1" style="1"/>
-    <col min="3" max="3" width="17.99" customWidth="1" style="2"/>
-    <col min="4" max="4" width="4.76" customWidth="1" style="1"/>
-    <col min="5" max="5" width="7.54" customWidth="1" style="1"/>
-    <col min="6" max="7" width="6.71" customWidth="1" style="1"/>
-    <col min="8" max="8" width="8.67" customWidth="1" style="3"/>
-    <col min="10" max="16384" width="11.52" customWidth="1" style="1"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="17.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -321,7 +345,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" ht="12.8">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -347,17 +371,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" ht="12.8">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="4" t="n">
         <v>31213</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="n">
         <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -369,8 +393,8 @@
       <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5">
-        <f>FALSE()</f>
+      <c r="H3" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
@@ -383,9 +407,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=EPPlusLicense.txt>This workbook was created with the EPPlus library, licensed to Ryan Weavers under the Polyform Noncommercial license, see https://polyformproject.org/licenses/noncommercial/1.0.0
-For more information about EPPlus, see https://epplussoftware.com/
-
 </file>
</xml_diff>